<commit_message>
Subida MAC y ARP
</commit_message>
<xml_diff>
--- a/Tabla_Ataques_MITRE-pcaps.xlsx
+++ b/Tabla_Ataques_MITRE-pcaps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cozas\Universidad\TFG_Seguridad_LAN\Mis notas\MITRE_PCAPS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A94E9C-26A5-4262-943E-949E32C07E05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9C22721-A2CA-413B-93E1-FB799C49A807}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="173">
   <si>
     <t>Reconnaissance</t>
   </si>
@@ -518,24 +518,44 @@
   </si>
   <si>
     <t>T1499_dhcp_flood.pcapng</t>
+  </si>
+  <si>
+    <t>Inundación MAC</t>
+  </si>
+  <si>
+    <t>macof</t>
+  </si>
+  <si>
+    <t>Suplantación MAC</t>
+  </si>
+  <si>
+    <t>ip (configuración)</t>
+  </si>
+  <si>
+    <t>Suplantación ARP</t>
+  </si>
+  <si>
+    <t>T1499_mac_spoof.pcapng</t>
+  </si>
+  <si>
+    <t>arpspoof</t>
+  </si>
+  <si>
+    <t>T1557_arp_spoof.pcapng</t>
+  </si>
+  <si>
+    <t>T1040_mac_flood.pcapng</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -561,18 +581,6 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -627,18 +635,12 @@
       <name val="Times"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -685,77 +687,56 @@
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="3" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="4" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="13" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
   </cellXfs>
@@ -982,8 +963,8 @@
   </sheetPr>
   <dimension ref="A1:H123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -993,1770 +974,1533 @@
     <col min="3" max="3" width="18.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="27.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="24.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="40" style="15" customWidth="1"/>
+    <col min="6" max="6" width="40" style="10" customWidth="1"/>
     <col min="7" max="7" width="28" style="1" customWidth="1"/>
-    <col min="8" max="8" width="33.140625" style="22" customWidth="1"/>
+    <col min="8" max="8" width="33.140625" style="16" customWidth="1"/>
     <col min="9" max="9" width="29.7109375" style="1" customWidth="1"/>
     <col min="10" max="10" width="11.42578125" style="1" customWidth="1"/>
     <col min="11" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="12" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" s="17" t="s">
+      <c r="D5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G5" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="H2" s="19" t="s">
+      <c r="H5" s="13" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
+    <row r="6" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="17" t="s">
+      <c r="D6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G6" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="H3" s="20" t="s">
+      <c r="H6" s="14" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
+    <row r="7" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B7" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C7" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="17" t="s">
+      <c r="D7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G7" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="H4" s="20" t="s">
+      <c r="H7" s="14" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
+    <row r="8" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B8" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C8" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D8" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E8" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F8" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="G5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" s="24" t="s">
+      <c r="G8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="17" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
+    <row r="9" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F9" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="G6" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H6" s="24" t="s">
+      <c r="G9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" s="17" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
+    <row r="10" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C10" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D10" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E10" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F10" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="G7" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H7" s="24" t="s">
+      <c r="G10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="17" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
+    <row r="11" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C11" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D11" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E11" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F8" s="17" t="s">
+      <c r="F11" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G11" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H8" s="20" t="s">
+      <c r="H11" s="14" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
+    <row r="12" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B12" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C12" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="17" t="s">
+      <c r="D12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G12" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="H9" s="20" t="s">
+      <c r="H12" s="14" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
+    <row r="13" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B13" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C13" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D13" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E13" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="17" t="s">
+      <c r="F13" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="G10" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H10" s="24" t="s">
+      <c r="G13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H13" s="17" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
+    <row r="14" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B14" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C14" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D14" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E14" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="17" t="s">
+      <c r="F14" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="G11" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H11" s="24" t="s">
+      <c r="G14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H14" s="17" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
+    <row r="15" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B15" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C15" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D15" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E15" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F12" s="17" t="s">
+      <c r="F15" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="G12" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H12" s="24" t="s">
+      <c r="G15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H15" s="17" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
+    <row r="16" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B16" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C16" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D16" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E16" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F13" s="17" t="s">
+      <c r="F16" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="G13" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H13" s="24" t="s">
+      <c r="G16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H16" s="17" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="7" t="s">
+    <row r="17" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B17" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C17" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D17" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="E17" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F14" s="17" t="s">
+      <c r="F17" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="G14" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H14" s="24" t="s">
+      <c r="G17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H17" s="17" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="7" t="s">
+    <row r="18" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B18" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C18" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D18" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E18" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F15" s="17" t="s">
+      <c r="F18" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="G15" s="7" t="s">
+      <c r="G18" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H15" s="20" t="s">
+      <c r="H18" s="14" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="7" t="s">
+    <row r="19" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B19" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C19" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D19" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="E19" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F16" s="17" t="s">
+      <c r="F19" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="G16" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H16" s="24" t="s">
+      <c r="G19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H19" s="17" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="7" t="s">
+    <row r="20" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B20" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C20" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D20" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E20" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F17" s="17" t="s">
+      <c r="F20" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="G17" s="7" t="s">
+      <c r="G20" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H17" s="20" t="s">
+      <c r="H20" s="14" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="7" t="s">
+    <row r="21" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B21" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C21" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D21" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="E21" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F18" s="17" t="s">
+      <c r="F21" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="G18" s="7" t="s">
+      <c r="G21" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H18" s="20" t="s">
+      <c r="H21" s="14" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="7" t="s">
+    <row r="22" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B22" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C22" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F19" s="17" t="s">
+      <c r="D22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F22" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="G19" s="7" t="s">
+      <c r="G22" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="H19" s="21" t="s">
+      <c r="H22" s="15" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="7" t="s">
+    <row r="23" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B23" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C23" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D20" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F20" s="17" t="s">
+      <c r="D23" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F23" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="G20" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H20" s="24" t="s">
+      <c r="G23" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H23" s="17" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="7" t="s">
+    <row r="24" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B24" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C24" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D24" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E21" s="8" t="s">
+      <c r="E24" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F21" s="17" t="s">
+      <c r="F24" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="G21" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H21" s="24" t="s">
+      <c r="G24" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H24" s="17" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="7" t="s">
+    <row r="25" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B25" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C25" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D25" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="E25" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F22" s="17" t="s">
+      <c r="F25" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="G22" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H22" s="24" t="s">
+      <c r="G25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H25" s="17" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="7" t="s">
+    <row r="26" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B26" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="C26" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D26" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E23" s="8" t="s">
+      <c r="E26" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F23" s="17" t="s">
+      <c r="F26" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="G23" s="7" t="s">
+      <c r="G26" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H23" s="20" t="s">
+      <c r="H26" s="14" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="7" t="s">
+    <row r="27" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B27" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C27" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D27" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E24" s="8" t="s">
+      <c r="E27" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F24" s="17" t="s">
+      <c r="F27" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="G24" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H24" s="24" t="s">
+      <c r="G27" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H27" s="17" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="7" t="s">
+    <row r="28" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B28" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C28" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D28" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E25" s="8" t="s">
+      <c r="E28" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="F25" s="17" t="s">
+      <c r="F28" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="G25" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H25" s="24" t="s">
+      <c r="G28" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H28" s="17" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="7" t="s">
+    <row r="29" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B29" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C29" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D29" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E26" s="8" t="s">
+      <c r="E29" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="F26" s="17" t="s">
+      <c r="F29" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="G26" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H26" s="24" t="s">
+      <c r="G29" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H29" s="17" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="7" t="s">
+    <row r="30" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="B30" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="C30" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D30" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E27" s="8" t="s">
+      <c r="E30" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F27" s="17" t="s">
+      <c r="F30" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="G27" s="7" t="s">
+      <c r="G30" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="H27" s="20" t="s">
+      <c r="H30" s="14" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="7" t="s">
+    <row r="31" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B31" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C31" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D28" s="7" t="s">
+      <c r="D31" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E28" s="8" t="s">
+      <c r="E31" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="F28" s="17" t="s">
+      <c r="F31" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="G28" s="7" t="s">
+      <c r="G31" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="H28" s="20" t="s">
+      <c r="H31" s="14" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="7" t="s">
+    <row r="32" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B32" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="C32" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="D32" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E29" s="8" t="s">
+      <c r="E32" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="F29" s="17" t="s">
+      <c r="F32" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="G29" s="7" t="s">
+      <c r="G32" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="H29" s="20" t="s">
+      <c r="H32" s="14" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="7" t="s">
+    <row r="33" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="B33" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="C33" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D30" s="7" t="s">
+      <c r="D33" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E30" s="8" t="s">
+      <c r="E33" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="F30" s="17" t="s">
+      <c r="F33" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="G30" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H30" s="24" t="s">
+      <c r="G33" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H33" s="17" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="10" t="s">
+    <row r="34" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="B34" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="C34" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D31" s="10" t="s">
+      <c r="D34" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E31" s="11" t="s">
+      <c r="E34" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F31" s="17" t="s">
+      <c r="F34" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="G31" s="12" t="s">
+      <c r="G34" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H31" s="20" t="s">
+      <c r="H34" s="14" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="7" t="s">
+    <row r="35" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B32" s="7" t="s">
+      <c r="B35" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C35" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D32" s="7" t="s">
+      <c r="D35" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E32" s="8" t="s">
+      <c r="E35" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="F32" s="17" t="s">
+      <c r="F35" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="G32" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H32" s="24" t="s">
+      <c r="G35" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H35" s="17" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="10" t="s">
+    <row r="36" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B36" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="C36" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="D36" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E33" s="8" t="s">
+      <c r="E36" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F33" s="17" t="s">
+      <c r="F36" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="G33" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H33" s="24" t="s">
+      <c r="G36" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H36" s="17" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="7" t="s">
+    <row r="37" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="B37" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="C37" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D34" s="7" t="s">
+      <c r="D37" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E34" s="8" t="s">
+      <c r="E37" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="F34" s="8" t="s">
+      <c r="F37" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="G34" s="8" t="s">
+      <c r="G37" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="H34" s="20" t="s">
+      <c r="H37" s="14" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="7" t="s">
+    <row r="38" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B38" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C35" s="9" t="s">
+      <c r="C38" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D35" s="7" t="s">
+      <c r="D38" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="E35" s="9" t="s">
+      <c r="E38" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="F35" s="7" t="s">
+      <c r="F38" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="G35" s="7" t="s">
+      <c r="G38" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="H35" s="9" t="s">
+      <c r="H38" s="4" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="7" t="s">
+    <row r="39" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="B39" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C36" s="8" t="s">
+      <c r="C39" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="D36" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E36" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F36" s="17" t="s">
+      <c r="D39" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F39" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="G36" s="7" t="s">
+      <c r="G39" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="H36" s="21" t="s">
+      <c r="H39" s="15" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="7" t="s">
+    <row r="40" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B37" s="7" t="s">
+      <c r="B40" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C37" s="8" t="s">
+      <c r="C40" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="D37" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E37" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F37" s="17" t="s">
+      <c r="D40" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F40" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="G37" s="7" t="s">
+      <c r="G40" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="H37" s="19" t="s">
+      <c r="H40" s="13" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="7" t="s">
+    <row r="41" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B38" s="7" t="s">
+      <c r="B41" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C38" s="8" t="s">
+      <c r="C41" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="D38" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E38" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F38" s="17" t="s">
+      <c r="D41" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F41" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="G38" s="7" t="s">
+      <c r="G41" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="H38" s="19" t="s">
+      <c r="H41" s="13" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="7" t="s">
+    <row r="42" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B39" s="7" t="s">
+      <c r="B42" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C39" s="8" t="s">
+      <c r="C42" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D39" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E39" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F39" s="17" t="s">
+      <c r="D42" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F42" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="G39" s="7" t="s">
+      <c r="G42" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="H39" s="21" t="s">
+      <c r="H42" s="15" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="7" t="s">
+    <row r="43" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B40" s="7" t="s">
+      <c r="B43" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C40" s="8" t="s">
+      <c r="C43" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D40" s="7" t="s">
+      <c r="D43" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E40" s="8" t="s">
+      <c r="E43" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="F40" s="17" t="s">
+      <c r="F43" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="G40" s="7" t="s">
+      <c r="G43" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="H40" s="21" t="s">
+      <c r="H43" s="15" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="7" t="s">
+    <row r="44" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B41" s="7" t="s">
+      <c r="B44" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C41" s="8" t="s">
+      <c r="C44" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D41" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E41" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F41" s="17" t="s">
+      <c r="D44" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F44" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="G41" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H41" s="24" t="s">
+      <c r="G44" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H44" s="17" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="7" t="s">
+    <row r="45" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B42" s="7" t="s">
+      <c r="B45" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C42" s="8" t="s">
+      <c r="C45" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D42" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E42" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F42" s="17" t="s">
+      <c r="D45" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F45" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="G42" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H42" s="24" t="s">
+      <c r="G45" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H45" s="17" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="7" t="s">
+    <row r="46" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B43" s="7" t="s">
+      <c r="B46" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C43" s="8" t="s">
+      <c r="C46" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D43" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E43" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F43" s="17" t="s">
+      <c r="D46" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F46" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="G43" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H43" s="24" t="s">
+      <c r="G46" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H46" s="17" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="7" t="s">
+    <row r="47" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B44" s="7" t="s">
+      <c r="B47" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C44" s="8" t="s">
+      <c r="C47" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="D44" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E44" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F44" s="17" t="s">
+      <c r="D47" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F47" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="G44" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H44" s="24" t="s">
+      <c r="G47" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H47" s="17" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="7" t="s">
+    <row r="48" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B45" s="7" t="s">
+      <c r="B48" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C45" s="8" t="s">
+      <c r="C48" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D45" s="7" t="s">
+      <c r="D48" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E45" s="8" t="s">
+      <c r="E48" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="F45" s="17" t="s">
+      <c r="F48" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="G45" s="13" t="s">
+      <c r="G48" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="H45" s="21" t="s">
+      <c r="H48" s="15" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="7" t="s">
+    <row r="49" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B46" s="7" t="s">
+      <c r="B49" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C46" s="8" t="s">
+      <c r="C49" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D46" s="7" t="s">
+      <c r="D49" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E46" s="8" t="s">
+      <c r="E49" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="F46" s="17" t="s">
+      <c r="F49" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="G46" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H46" s="24" t="s">
+      <c r="G49" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H49" s="17" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="7" t="s">
+    <row r="50" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B47" s="7" t="s">
+      <c r="B50" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C47" s="8" t="s">
+      <c r="C50" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D47" s="7" t="s">
+      <c r="D50" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E47" s="8" t="s">
+      <c r="E50" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="F47" s="17" t="s">
+      <c r="F50" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="G47" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H47" s="24" t="s">
+      <c r="G50" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H50" s="17" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="7" t="s">
+    <row r="51" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B48" s="7" t="s">
+      <c r="B51" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C48" s="8" t="s">
+      <c r="C51" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D48" s="7" t="s">
+      <c r="D51" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E48" s="8" t="s">
+      <c r="E51" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F48" s="17" t="s">
+      <c r="F51" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="G48" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H48" s="24" t="s">
+      <c r="G51" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H51" s="17" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="7" t="s">
+    <row r="52" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B49" s="7" t="s">
+      <c r="B52" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C49" s="8" t="s">
+      <c r="C52" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D49" s="7" t="s">
+      <c r="D52" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E49" s="8" t="s">
+      <c r="E52" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="F49" s="17" t="s">
+      <c r="F52" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="G49" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H49" s="24" t="s">
+      <c r="G52" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H52" s="17" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="7" t="s">
+    <row r="53" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B50" s="7" t="s">
+      <c r="B53" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C50" s="8" t="s">
+      <c r="C53" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D50" s="7" t="s">
+      <c r="D53" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E50" s="8" t="s">
+      <c r="E53" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="F50" s="17" t="s">
+      <c r="F53" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="G50" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H50" s="24" t="s">
+      <c r="G53" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H53" s="17" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="7" t="s">
+    <row r="54" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B51" s="7" t="s">
+      <c r="B54" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C51" s="8" t="s">
+      <c r="C54" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D51" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E51" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F51" s="17" t="s">
+      <c r="D54" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F54" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="G51" s="7" t="s">
+      <c r="G54" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="H51" s="20" t="s">
+      <c r="H54" s="14" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="7" t="s">
+    <row r="55" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B52" s="7" t="s">
+      <c r="B55" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C52" s="8" t="s">
+      <c r="C55" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D52" s="7" t="s">
+      <c r="D55" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E52" s="8" t="s">
+      <c r="E55" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="F52" s="17" t="s">
+      <c r="F55" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="G52" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H52" s="24" t="s">
+      <c r="G55" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H55" s="17" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="7" t="s">
+    <row r="56" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B53" s="7" t="s">
+      <c r="B56" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C53" s="7" t="s">
+      <c r="C56" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D53" s="7" t="s">
+      <c r="D56" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E53" s="8" t="s">
+      <c r="E56" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F53" s="17" t="s">
+      <c r="F56" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="G53" s="7" t="s">
+      <c r="G56" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="H53" s="21" t="s">
+      <c r="H56" s="15" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="7" t="s">
+    <row r="57" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B54" s="7" t="s">
+      <c r="B57" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C54" s="9" t="s">
+      <c r="C57" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D54" s="7" t="s">
+      <c r="D57" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E54" s="8" t="s">
+      <c r="E57" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F54" s="17" t="s">
+      <c r="F57" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="G54" s="7" t="s">
+      <c r="G57" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="H54" s="20" t="s">
+      <c r="H57" s="14" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A89" s="5"/>
-      <c r="B89" s="5"/>
-      <c r="C89" s="5"/>
-      <c r="D89" s="5"/>
-      <c r="E89" s="5"/>
-      <c r="F89" s="16"/>
-      <c r="G89" s="2"/>
-      <c r="H89" s="23"/>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A90" s="4"/>
-      <c r="B90" s="4"/>
-      <c r="C90" s="5"/>
-      <c r="D90" s="4"/>
-      <c r="E90" s="5"/>
-      <c r="F90" s="16"/>
-      <c r="G90" s="2"/>
-      <c r="H90" s="23"/>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A91" s="5"/>
-      <c r="B91" s="5"/>
-      <c r="C91" s="5"/>
-      <c r="D91" s="5"/>
-      <c r="E91" s="5"/>
-      <c r="F91" s="16"/>
-      <c r="G91" s="2"/>
-      <c r="H91" s="23"/>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A92" s="4"/>
-      <c r="B92" s="4"/>
-      <c r="C92" s="5"/>
-      <c r="D92" s="4"/>
-      <c r="E92" s="5"/>
-      <c r="F92" s="16"/>
-      <c r="G92" s="2"/>
-      <c r="H92" s="23"/>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A93" s="5"/>
-      <c r="B93" s="5"/>
-      <c r="C93" s="5"/>
-      <c r="D93" s="5"/>
-      <c r="E93" s="5"/>
-      <c r="F93" s="16"/>
-      <c r="G93" s="2"/>
-      <c r="H93" s="23"/>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A94" s="4"/>
-      <c r="B94" s="4"/>
-      <c r="C94" s="5"/>
-      <c r="D94" s="3"/>
-      <c r="E94" s="3"/>
-      <c r="F94" s="16"/>
-      <c r="G94" s="2"/>
-      <c r="H94" s="23"/>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A95" s="4"/>
-      <c r="B95" s="4"/>
-      <c r="C95" s="5"/>
-      <c r="D95" s="4"/>
-      <c r="E95" s="5"/>
-      <c r="F95" s="16"/>
-      <c r="G95" s="2"/>
-      <c r="H95" s="23"/>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A96" s="5"/>
-      <c r="B96" s="5"/>
-      <c r="C96" s="5"/>
-      <c r="D96" s="3"/>
-      <c r="E96" s="3"/>
-      <c r="F96" s="16"/>
-      <c r="G96" s="2"/>
-      <c r="H96" s="23"/>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A97" s="4"/>
-      <c r="B97" s="4"/>
-      <c r="C97" s="5"/>
-      <c r="D97" s="3"/>
-      <c r="E97" s="3"/>
-      <c r="F97" s="16"/>
-      <c r="G97" s="2"/>
-      <c r="H97" s="23"/>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A98" s="5"/>
-      <c r="B98" s="5"/>
-      <c r="C98" s="5"/>
-      <c r="D98" s="5"/>
-      <c r="E98" s="5"/>
-      <c r="F98" s="16"/>
-      <c r="G98" s="6"/>
-      <c r="H98" s="23"/>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A99" s="4"/>
-      <c r="B99" s="4"/>
-      <c r="C99" s="5"/>
-      <c r="D99" s="4"/>
-      <c r="E99" s="5"/>
-      <c r="F99" s="16"/>
-      <c r="G99" s="2"/>
-      <c r="H99" s="23"/>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A100" s="5"/>
-      <c r="B100" s="5"/>
-      <c r="C100" s="5"/>
-      <c r="D100" s="5"/>
-      <c r="E100" s="5"/>
-      <c r="F100" s="16"/>
-      <c r="G100" s="2"/>
-      <c r="H100" s="23"/>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A101" s="5"/>
-      <c r="B101" s="5"/>
-      <c r="C101" s="5"/>
-      <c r="D101" s="5"/>
-      <c r="E101" s="5"/>
-      <c r="F101" s="16"/>
-      <c r="G101" s="2"/>
-      <c r="H101" s="23"/>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A102" s="4"/>
-      <c r="B102" s="4"/>
-      <c r="C102" s="5"/>
-      <c r="D102" s="4"/>
-      <c r="E102" s="5"/>
-      <c r="F102" s="16"/>
-      <c r="G102" s="2"/>
-      <c r="H102" s="23"/>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A103" s="4"/>
-      <c r="B103" s="4"/>
-      <c r="C103" s="5"/>
-      <c r="D103" s="4"/>
-      <c r="E103" s="5"/>
-      <c r="F103" s="16"/>
-      <c r="G103" s="2"/>
-      <c r="H103" s="23"/>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A104" s="4"/>
-      <c r="B104" s="4"/>
-      <c r="C104" s="5"/>
-      <c r="D104" s="4"/>
-      <c r="E104" s="5"/>
-      <c r="F104" s="16"/>
-      <c r="G104" s="2"/>
-      <c r="H104" s="23"/>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A105" s="5"/>
-      <c r="B105" s="5"/>
-      <c r="C105" s="5"/>
-      <c r="D105" s="3"/>
-      <c r="E105" s="3"/>
-      <c r="F105" s="16"/>
-      <c r="G105" s="2"/>
-      <c r="H105" s="23"/>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A106" s="5"/>
-      <c r="B106" s="5"/>
-      <c r="C106" s="5"/>
-      <c r="D106" s="5"/>
-      <c r="E106" s="5"/>
-      <c r="F106" s="16"/>
-      <c r="G106" s="2"/>
-      <c r="H106" s="23"/>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A107" s="4"/>
-      <c r="B107" s="4"/>
-      <c r="C107" s="5"/>
-      <c r="D107" s="4"/>
-      <c r="E107" s="5"/>
-      <c r="F107" s="16"/>
-      <c r="G107" s="2"/>
-      <c r="H107" s="23"/>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A108" s="4"/>
-      <c r="B108" s="4"/>
-      <c r="C108" s="5"/>
-      <c r="D108" s="4"/>
-      <c r="E108" s="5"/>
-      <c r="F108" s="16"/>
-      <c r="G108" s="2"/>
-      <c r="H108" s="23"/>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A109" s="4"/>
-      <c r="B109" s="4"/>
-      <c r="C109" s="5"/>
-      <c r="D109" s="4"/>
-      <c r="E109" s="5"/>
-      <c r="F109" s="16"/>
-      <c r="G109" s="2"/>
-      <c r="H109" s="23"/>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A110" s="4"/>
-      <c r="B110" s="4"/>
-      <c r="C110" s="5"/>
-      <c r="D110" s="3"/>
-      <c r="E110" s="3"/>
-      <c r="F110" s="16"/>
-      <c r="G110" s="2"/>
-      <c r="H110" s="23"/>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A111" s="4"/>
-      <c r="B111" s="4"/>
-      <c r="C111" s="5"/>
-      <c r="D111" s="4"/>
-      <c r="E111" s="5"/>
-      <c r="F111" s="16"/>
-      <c r="G111" s="2"/>
-      <c r="H111" s="23"/>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A112" s="4"/>
-      <c r="B112" s="4"/>
-      <c r="C112" s="5"/>
-      <c r="D112" s="3"/>
-      <c r="E112" s="3"/>
-      <c r="F112" s="16"/>
-      <c r="G112" s="2"/>
-      <c r="H112" s="23"/>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A113" s="5"/>
-      <c r="B113" s="5"/>
-      <c r="C113" s="5"/>
-      <c r="D113" s="5"/>
-      <c r="E113" s="5"/>
-      <c r="F113" s="16"/>
-      <c r="G113" s="2"/>
-      <c r="H113" s="23"/>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A114" s="4"/>
-      <c r="B114" s="4"/>
-      <c r="C114" s="5"/>
-      <c r="D114" s="4"/>
-      <c r="E114" s="5"/>
-      <c r="F114" s="16"/>
-      <c r="G114" s="2"/>
-      <c r="H114" s="23"/>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A115" s="5"/>
-      <c r="B115" s="5"/>
-      <c r="C115" s="5"/>
-      <c r="D115" s="5"/>
-      <c r="E115" s="5"/>
-      <c r="F115" s="16"/>
-      <c r="G115" s="2"/>
-      <c r="H115" s="23"/>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A116" s="4"/>
-      <c r="B116" s="4"/>
-      <c r="C116" s="5"/>
-      <c r="D116" s="3"/>
-      <c r="E116" s="3"/>
-      <c r="F116" s="16"/>
-      <c r="G116" s="2"/>
-      <c r="H116" s="23"/>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A117" s="4"/>
-      <c r="B117" s="4"/>
-      <c r="C117" s="5"/>
-      <c r="D117" s="3"/>
-      <c r="E117" s="3"/>
-      <c r="F117" s="16"/>
-      <c r="G117" s="2"/>
-      <c r="H117" s="23"/>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A118" s="5"/>
-      <c r="B118" s="5"/>
-      <c r="C118" s="5"/>
-      <c r="D118" s="3"/>
-      <c r="E118" s="3"/>
-      <c r="F118" s="16"/>
-      <c r="G118" s="2"/>
-      <c r="H118" s="23"/>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A119" s="5"/>
-      <c r="B119" s="4"/>
-      <c r="C119" s="5"/>
-      <c r="D119" s="3"/>
-      <c r="E119" s="3"/>
-      <c r="F119" s="16"/>
-      <c r="G119" s="2"/>
-      <c r="H119" s="23"/>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A120" s="5"/>
-      <c r="B120" s="5"/>
-      <c r="C120" s="5"/>
-      <c r="D120" s="3"/>
-      <c r="E120" s="3"/>
-      <c r="F120" s="16"/>
-      <c r="G120" s="2"/>
-      <c r="H120" s="23"/>
-    </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A121" s="4"/>
-      <c r="B121" s="4"/>
-      <c r="C121" s="5"/>
-      <c r="D121" s="4"/>
-      <c r="E121" s="5"/>
-      <c r="F121" s="16"/>
-      <c r="G121" s="2"/>
-      <c r="H121" s="23"/>
-    </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A122" s="5"/>
-      <c r="B122" s="5"/>
-      <c r="C122" s="5"/>
-      <c r="D122" s="4"/>
-      <c r="E122" s="5"/>
-      <c r="F122" s="16"/>
-      <c r="G122" s="2"/>
-      <c r="H122" s="23"/>
-    </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A123" s="5"/>
-      <c r="B123" s="5"/>
-      <c r="C123" s="5"/>
-      <c r="D123" s="3"/>
-      <c r="E123" s="3"/>
-      <c r="F123" s="16"/>
-      <c r="G123" s="2"/>
-      <c r="H123" s="23"/>
-    </row>
+    <row r="89" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2"/>
+    <row r="90" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2"/>
+    <row r="91" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2"/>
+    <row r="92" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2"/>
+    <row r="93" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2"/>
+    <row r="94" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2"/>
+    <row r="95" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2"/>
+    <row r="96" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2"/>
+    <row r="97" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2"/>
+    <row r="98" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2"/>
+    <row r="99" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2"/>
+    <row r="100" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2"/>
+    <row r="101" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2"/>
+    <row r="102" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2"/>
+    <row r="103" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2"/>
+    <row r="104" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2"/>
+    <row r="105" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2"/>
+    <row r="106" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2"/>
+    <row r="107" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2"/>
+    <row r="108" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2"/>
+    <row r="109" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2"/>
+    <row r="110" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2"/>
+    <row r="111" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2"/>
+    <row r="112" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2"/>
+    <row r="113" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2"/>
+    <row r="114" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2"/>
+    <row r="115" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2"/>
+    <row r="116" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2"/>
+    <row r="117" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2"/>
+    <row r="118" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2"/>
+    <row r="119" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2"/>
+    <row r="120" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2"/>
+    <row r="121" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2"/>
+    <row r="122" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2"/>
+    <row r="123" s="1" customFormat="1" ht="14.25" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>